<commit_message>
YET another update TEXT CHANGE
</commit_message>
<xml_diff>
--- a/mappings/package_F03_test/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03_test/transformation/conceptual_mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="546">
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -2763,16 +2763,10 @@
     <t xml:space="preserve">main_activity.json</t>
   </si>
   <si>
-    <t xml:space="preserve">currency.json</t>
-  </si>
-  <si>
     <t xml:space="preserve">cpv.json</t>
   </si>
   <si>
     <t xml:space="preserve">contract_nature.json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buyer_main_activity.json</t>
   </si>
   <si>
     <t xml:space="preserve">buyer_legal_type.json</t>
@@ -3579,11 +3573,11 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
@@ -3697,7 +3691,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3705,16 +3699,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3742,7 +3736,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3750,16 +3744,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3787,7 +3781,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3795,16 +3789,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3832,7 +3826,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3840,16 +3834,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +3871,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3885,16 +3879,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3922,7 +3916,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16"/>
@@ -3951,7 +3945,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.22"/>
@@ -3960,7 +3954,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10275,13 +10269,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.79"/>
   </cols>
@@ -10316,7 +10310,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
         <v>507</v>
       </c>
@@ -10331,16 +10325,8 @@
         <v>509</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>511</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10363,7 +10349,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.78"/>
@@ -10371,62 +10357,62 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="50" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="53" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="53" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="54" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
       <c r="B11" s="55" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="56" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="57" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="58" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10435,7 +10421,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B16" s="44"/>
     </row>
@@ -10447,10 +10433,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="53" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -10475,7 +10461,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.66"/>
@@ -10586,25 +10572,25 @@
         <v>61</v>
       </c>
       <c r="D5" s="59" t="s">
+        <v>526</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="F5" s="60" t="s">
         <v>528</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="G5" s="60" t="s">
         <v>529</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="H5" s="61" t="s">
         <v>530</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="I5" s="59" t="s">
         <v>531</v>
       </c>
-      <c r="H5" s="61" t="s">
+      <c r="J5" s="60" t="s">
         <v>532</v>
-      </c>
-      <c r="I5" s="59" t="s">
-        <v>533</v>
-      </c>
-      <c r="J5" s="60" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10637,7 +10623,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -10645,40 +10631,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -10706,7 +10692,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -10714,32 +10700,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -10767,7 +10753,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -10775,16 +10761,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -10812,7 +10798,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -10820,16 +10806,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B1" s="62"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated resources list and version format
</commit_message>
<xml_diff>
--- a/mappings/package_F03_test/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03_test/transformation/conceptual_mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1</t>
+    <t xml:space="preserve">1.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">EPO version</t>
@@ -2751,16 +2751,16 @@
     <t xml:space="preserve">File name</t>
   </si>
   <si>
-    <t xml:space="preserve">countries.json</t>
+    <t xml:space="preserve">country.json</t>
   </si>
   <si>
     <t xml:space="preserve">nuts.json</t>
   </si>
   <si>
-    <t xml:space="preserve">procurement_procedure_type.json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main_activity.json</t>
+    <t xml:space="preserve">main_activity.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency.json</t>
   </si>
   <si>
     <t xml:space="preserve">cpv.json</t>
@@ -2769,7 +2769,7 @@
     <t xml:space="preserve">contract_nature.json</t>
   </si>
   <si>
-    <t xml:space="preserve">buyer_legal_type.json</t>
+    <t xml:space="preserve">buyer_legal_type.csv</t>
   </si>
   <si>
     <t xml:space="preserve">award_criterion_type.json</t>
@@ -3573,11 +3573,11 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
@@ -3691,7 +3691,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3736,7 +3736,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3781,7 +3781,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3826,7 +3826,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3871,7 +3871,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -3916,7 +3916,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16"/>
@@ -3945,7 +3945,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.22"/>
@@ -10271,11 +10271,11 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.79"/>
   </cols>
@@ -10295,7 +10295,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
         <v>504</v>
       </c>
@@ -10349,7 +10349,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.78"/>
@@ -10461,7 +10461,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.66"/>
@@ -10623,7 +10623,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -10692,7 +10692,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -10753,7 +10753,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -10798,7 +10798,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>

</xml_diff>